<commit_message>
added table creation - everything working, need more data
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="14200" windowHeight="16340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
   <si>
     <t>Chart</t>
   </si>
@@ -117,28 +117,55 @@
     <t>Grenville Orogeny (1350-1480)</t>
   </si>
   <si>
+    <t>Rodinia Supercontinent</t>
+  </si>
+  <si>
+    <t>Sturtian-Varangian Ice Age</t>
+  </si>
+  <si>
+    <t>1st Protozoa</t>
+  </si>
+  <si>
+    <t>"Snowball Earth"</t>
+  </si>
+  <si>
+    <t>Pan-African Orogeny (Gondwana &amp; Pannotia Supercontinents</t>
+  </si>
+  <si>
+    <t>Lantian formation Southern China</t>
+  </si>
+  <si>
+    <t>Tbl</t>
+  </si>
+  <si>
+    <t>Bogus1</t>
+  </si>
+  <si>
+    <t>Bogus3</t>
+  </si>
+  <si>
+    <t>Bogus2</t>
+  </si>
+  <si>
     <t>K</t>
   </si>
   <si>
-    <t>Rodinia Supercontinent</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
-    <t>Sturtian-Varangian Ice Age</t>
-  </si>
-  <si>
-    <t>1st Protozoa</t>
-  </si>
-  <si>
-    <t>"Snowball Earth"</t>
-  </si>
-  <si>
-    <t>Pan-African Orogeny (Gondwana &amp; Pannotia Supercontinents</t>
-  </si>
-  <si>
-    <t>Lantian formation Southern China</t>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Phanerozoic</t>
   </si>
 </sst>
 </file>
@@ -215,10 +242,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -560,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E25" sqref="E24:E25"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -635,7 +663,7 @@
         <v>4000</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -649,7 +677,7 @@
         <v>4000</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>14</v>
@@ -663,7 +691,7 @@
         <v>4000</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -677,7 +705,7 @@
         <v>4000</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -733,7 +761,7 @@
         <v>2500</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -747,7 +775,7 @@
         <v>2500</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>18</v>
@@ -761,7 +789,7 @@
         <v>2500</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
@@ -775,7 +803,7 @@
         <v>2500</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
         <v>18</v>
@@ -789,7 +817,7 @@
         <v>2400</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
@@ -803,7 +831,7 @@
         <v>1700</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
@@ -817,7 +845,7 @@
         <v>1670</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
         <v>27</v>
@@ -831,7 +859,7 @@
         <v>1500</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
         <v>29</v>
@@ -845,7 +873,7 @@
         <v>1480</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
         <v>31</v>
@@ -859,10 +887,10 @@
         <v>1000</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -873,10 +901,10 @@
         <v>800</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -887,10 +915,10 @@
         <v>750</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -901,10 +929,10 @@
         <v>650</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -915,10 +943,10 @@
         <v>600</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="1" customFormat="1">
@@ -929,10 +957,52 @@
         <v>541</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="3">
+        <v>400</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="3">
+        <v>300</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="3">
+        <v>200</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated events to include all clickables, and fixed minor typos and bugs
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="74">
   <si>
     <t>Chart</t>
   </si>
@@ -96,15 +96,9 @@
     <t>G</t>
   </si>
   <si>
-    <t>Oldest New Mexico Rocks</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
-    <t>Mazatzal Orogeny (1650-1670)</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
@@ -114,18 +108,12 @@
     <t>J</t>
   </si>
   <si>
-    <t>Grenville Orogeny (1350-1480)</t>
-  </si>
-  <si>
     <t>Rodinia Supercontinent</t>
   </si>
   <si>
     <t>Sturtian-Varangian Ice Age</t>
   </si>
   <si>
-    <t>1st Protozoa</t>
-  </si>
-  <si>
     <t>"Snowball Earth"</t>
   </si>
   <si>
@@ -138,9 +126,6 @@
     <t>Tbl</t>
   </si>
   <si>
-    <t>Bogus1</t>
-  </si>
-  <si>
     <t>Bogus3</t>
   </si>
   <si>
@@ -166,6 +151,96 @@
   </si>
   <si>
     <t>Phanerozoic</t>
+  </si>
+  <si>
+    <t>Single-celled life forms</t>
+  </si>
+  <si>
+    <t>Oldest New Mexico Rocks (Sangre de Cristos, Zuni &amp; Nacimientos)</t>
+  </si>
+  <si>
+    <t>Mazatzal Orogeny (1650-1670: Collisions w/Laurentia Continent)</t>
+  </si>
+  <si>
+    <t>Grenville Orogeny (1350-1480: Sandia Granite)</t>
+  </si>
+  <si>
+    <t>1st Protozoa/ Splitting up of Rodinia supercontinent</t>
+  </si>
+  <si>
+    <t>Paleozoic</t>
+  </si>
+  <si>
+    <t>Fragments from Rodinia breakup begin to re-merge</t>
+  </si>
+  <si>
+    <t>NM mostly 'quiet' and above sea level until Mississippian</t>
+  </si>
+  <si>
+    <t>Carboniferous</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>Sea begins to intrude into New Mexico/ Mississippian remnants at Gilman</t>
+  </si>
+  <si>
+    <t>Paleo</t>
+  </si>
+  <si>
+    <t>Any</t>
+  </si>
+  <si>
+    <t>Meso</t>
+  </si>
+  <si>
+    <t>Neo</t>
+  </si>
+  <si>
+    <t>Mesozoic</t>
+  </si>
+  <si>
+    <t>Cenozoic</t>
+  </si>
+  <si>
+    <t>Cambrian</t>
+  </si>
+  <si>
+    <t>Ordovician</t>
+  </si>
+  <si>
+    <t>Silurian</t>
+  </si>
+  <si>
+    <t>Devonian</t>
+  </si>
+  <si>
+    <t>Permian</t>
+  </si>
+  <si>
+    <t>Triassic</t>
+  </si>
+  <si>
+    <t>Jurassic</t>
+  </si>
+  <si>
+    <t>Cretaceous</t>
+  </si>
+  <si>
+    <t>Paleogene</t>
+  </si>
+  <si>
+    <t>Neogene</t>
+  </si>
+  <si>
+    <t>Quaternary</t>
+  </si>
+  <si>
+    <t>F--&gt;</t>
+  </si>
+  <si>
+    <t>1400 - 330MYA: The Great Unconformity (gap in rock record - Sandia)</t>
   </si>
 </sst>
 </file>
@@ -229,7 +304,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -241,24 +316,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -588,15 +668,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="4" width="51.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="4" max="4" width="57" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="18">
@@ -663,7 +744,7 @@
         <v>4000</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -677,7 +758,7 @@
         <v>4000</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>14</v>
@@ -691,7 +772,7 @@
         <v>4000</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -705,7 +786,7 @@
         <v>4000</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -716,13 +797,13 @@
         <v>22</v>
       </c>
       <c r="B9">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -730,13 +811,13 @@
         <v>22</v>
       </c>
       <c r="B10">
-        <v>2700</v>
+        <v>3500</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -747,10 +828,10 @@
         <v>2700</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -758,41 +839,41 @@
         <v>22</v>
       </c>
       <c r="B12">
+        <v>2700</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
         <v>2500</v>
       </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="1" customFormat="1">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:4" s="1" customFormat="1">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B14" s="1">
         <v>2500</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14">
-        <v>2500</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -803,10 +884,10 @@
         <v>2500</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -814,13 +895,13 @@
         <v>23</v>
       </c>
       <c r="B16">
-        <v>2400</v>
+        <v>2500</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -828,13 +909,13 @@
         <v>23</v>
       </c>
       <c r="B17">
-        <v>1700</v>
+        <v>2400</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -842,13 +923,13 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>1670</v>
+        <v>1750</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -856,13 +937,13 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>1500</v>
+        <v>1670</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -870,13 +951,13 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>1480</v>
+        <v>1500</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -884,13 +965,13 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>1000</v>
+        <v>1480</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -898,13 +979,13 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>800</v>
+        <v>1400</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -912,13 +993,13 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>750</v>
+        <v>1000</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -926,13 +1007,13 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>650</v>
+        <v>800</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -940,69 +1021,349 @@
         <v>23</v>
       </c>
       <c r="B25">
+        <v>750</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>650</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27">
         <v>600</v>
       </c>
-      <c r="C25" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="1" customFormat="1">
-      <c r="A26" s="1" t="s">
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="1" customFormat="1">
+      <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B28" s="1">
         <v>541</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="3">
-        <v>400</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="3">
-        <v>300</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>41</v>
+      <c r="C28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="3">
+        <v>541</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="3">
+        <v>300</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="1" customFormat="1">
+      <c r="A31" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="4">
+        <v>200</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="3">
+        <v>2050</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="3">
+        <v>1200</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="3">
+        <v>720</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="3">
+        <v>541</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="3">
+        <v>100.5</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="3">
+        <v>21</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="3">
+        <v>500</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="3">
+        <v>460</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="3">
+        <v>430</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="3">
+        <v>385</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="3">
+        <v>330</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" s="3">
+        <v>270</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="3">
+        <v>235</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="3">
+        <v>170</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="3">
+        <v>100</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B47" s="3">
         <v>48</v>
       </c>
-      <c r="B29" s="3">
-        <v>200</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>40</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" s="3">
+        <v>15</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B49" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed order of presentation: chart-table-breakdown; was breakdown-chart-table
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="67">
   <si>
     <t>Chart</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Pangola Ice Age</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>1st Major Ice Age (Huronian: 2100-2400)</t>
   </si>
   <si>
@@ -135,21 +132,6 @@
     <t>K</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>Phanerozoic</t>
   </si>
   <si>
@@ -178,9 +160,6 @@
   </si>
   <si>
     <t>Carboniferous</t>
-  </si>
-  <si>
-    <t>Q</t>
   </si>
   <si>
     <t>Sea begins to intrude into New Mexico/ Mississippian remnants at Gilman</t>
@@ -670,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -744,7 +723,7 @@
         <v>4000</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -758,7 +737,7 @@
         <v>4000</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>14</v>
@@ -766,13 +745,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>4000</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -780,13 +759,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>4000</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -794,21 +773,21 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>4000</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <v>3500</v>
@@ -822,7 +801,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>2700</v>
@@ -836,7 +815,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <v>2700</v>
@@ -850,13 +829,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>2500</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
         <v>17</v>
@@ -864,13 +843,13 @@
     </row>
     <row r="14" spans="1:4" s="1" customFormat="1">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1">
         <v>2500</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>18</v>
@@ -878,13 +857,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>2500</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -892,13 +871,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>2500</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -906,7 +885,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>2400</v>
@@ -915,12 +894,12 @@
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>1750</v>
@@ -929,12 +908,12 @@
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>1670</v>
@@ -943,12 +922,12 @@
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>1500</v>
@@ -957,12 +936,12 @@
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>1480</v>
@@ -971,152 +950,152 @@
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <v>1400</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>1000</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>800</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25">
         <v>750</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26">
         <v>650</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27">
         <v>600</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="1" customFormat="1">
       <c r="A28" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="1">
         <v>541</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B29" s="3">
         <v>541</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B30" s="3">
         <v>300</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="1" customFormat="1">
       <c r="A31" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B31" s="4">
         <v>200</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B32" s="3">
         <v>2050</v>
@@ -1125,12 +1104,12 @@
         <v>8</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B33" s="3">
         <v>1200</v>
@@ -1139,12 +1118,12 @@
         <v>7</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B34" s="3">
         <v>720</v>
@@ -1153,217 +1132,217 @@
         <v>5</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B35" s="3">
         <v>541</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B36" s="3">
         <v>100.5</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B37" s="3">
         <v>21</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B38" s="3">
         <v>500</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B39" s="3">
         <v>460</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B40" s="3">
         <v>430</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B41" s="3">
         <v>385</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B42" s="3">
         <v>330</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B43" s="3">
         <v>270</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B44" s="3">
         <v>235</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B45" s="3">
         <v>170</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B46" s="3">
         <v>100</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B47" s="3">
         <v>48</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B48" s="3">
         <v>15</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B49" s="3">
         <v>0.5</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>